<commit_message>
Change func of measure time
changed chrono::high_resolution_clock::now(); to omp_get_wtime(); and updated grafico.xlsx with new data
</commit_message>
<xml_diff>
--- a/taller 3/grafico.xlsx
+++ b/taller 3/grafico.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
   <si>
     <t>Secuencial</t>
   </si>
@@ -77,6 +77,12 @@
   <si>
     <t>Speed UP</t>
   </si>
+  <si>
+    <t>Windows primer FOR con omp_get_wtime()</t>
+  </si>
+  <si>
+    <t>Windows primer FOR con chrono</t>
+  </si>
 </sst>
 </file>
 
@@ -115,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -140,6 +146,9 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -226,7 +235,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4989,6 +4997,617 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>OpenMP - Windows primer for parralel - Completa - SpeedUp - omp_get_wtime()</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$D$436</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Speed UP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja1!$A$437:$A$473</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$D$437:$D$473</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.24997025139818427</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.24997025139818427</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.60003819912142009</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.50000012499415658</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.0000475989052331</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.83337972373763547</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.0001428103109125</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.4000948868508305</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.4284937573988885</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.5000990032341055</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.7500450005850077</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.8000281735812611</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.6800215169239374</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.4074096063141184</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.8371993280388033</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.007417517384873</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.9629667319986588</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.8605398394250461</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.7872364142153616</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.2565336291232363</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.435234135205179</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.3040334931455693</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6.0810142531478641</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.6528863650361494</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.3413462493733688</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5.4406696278792657</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5.1429074951843656</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.6908288932129256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CFDF-4FB8-9982-B60AD39A6086}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1000899568"/>
+        <c:axId val="1000911216"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1000899568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1000911216"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1000911216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1000899568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -5096,7 +5715,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10273,7 +10891,6 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10369,7 +10986,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10444,7 +11060,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10551,7 +11166,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14042,7 +14656,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -14149,7 +14762,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -14224,7 +14836,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14336,7 +14947,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -19480,7 +20090,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -19562,7 +20171,6 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -19637,7 +20245,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -19744,7 +20351,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -23242,7 +23848,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -23324,7 +23929,6 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -23399,7 +24003,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -23506,7 +24109,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -25863,7 +26465,6 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -25959,7 +26560,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -26034,7 +26634,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -26140,7 +26739,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>MP - Windows primer for parralel - Completa</a:t>
+              <a:t>MP - Windows primer for parralel - Completa - Rendimiento - chrono</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -27463,6 +28062,56 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>OpenMP - Windows primer for parralel - Completa</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t> - SpeedUp - Chrono</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -27476,13 +28125,27 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
-                </a:schemeClr>
+                </a:sysClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -27971,6 +28634,891 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>OpenMP - Windows primer for parralel - Completa - ome_get_wtime()</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$B$436</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tiempo Secuencial</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja1!$A$437:$A$473</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$437:$B$473</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.4998199999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.4998199999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.5006499999999995E-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.000235E-4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.25008825E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.2500287499999901E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.25008825E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.74999225E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.4999380000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.2500749999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.5000445000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.4249980250000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.9249965999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.9499919499999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.10400003225</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.16900002949999901</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.26800000624999998</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.49374997599999898</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.61200004824999998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.80424994225000002</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.0489999652499999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.28225010625</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.8015000225</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.1537499425000002</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.4997500179999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.0032498834999899</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.62575000525</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.3065000177499897</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7E87-4D8A-85E0-33060AAD2941}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$C$436</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tiempo Paralelo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja1!$A$437:$A$473</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$C$437:$C$473</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>1.2500287500000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.000047E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.5000549999999896E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.499951E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.9992774999999902E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.9998749999999901E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.9992799999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.9998749999999901E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.000047E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.000047E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.999875000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.2500287500000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.0000467499999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.2500287499999901E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.499951E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.2499097499999901E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.24990975E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7500517499999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.499951E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9999739999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.7499669999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.2499640000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.34999749999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.1500050999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.374993775E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.3999960249999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8.4249913750000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.105749965</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.15300005649999901</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.192999959</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.24175000175</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.296249926</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.38100004199999998</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.467999994999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.55200004574999995</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.70500004299999997</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.13124996425</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7E87-4D8A-85E0-33060AAD2941}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1101303488"/>
+        <c:axId val="1101305152"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1101303488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1101305152"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1101305152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1101303488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -28249,6 +29797,86 @@
 </file>
 
 <file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -31809,6 +33437,1025 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -32046,6 +34693,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>716280</xdr:colOff>
+      <xdr:row>452</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>487</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Gráfico 10"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>701040</xdr:colOff>
+      <xdr:row>490</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>522</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Gráfico 11"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -32317,10 +35024,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S431"/>
+  <dimension ref="A1:S473"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A389" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="G423" sqref="G423"/>
+    <sheetView tabSelected="1" topLeftCell="A469" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="AA497" sqref="AA497"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -51444,13 +54151,22 @@
       <c r="G379" s="5"/>
     </row>
     <row r="380" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A380" s="2" t="s">
+      <c r="A380" s="13" t="s">
         <v>17</v>
       </c>
+      <c r="B380" s="13"/>
+      <c r="C380" s="13"/>
+      <c r="D380" s="13"/>
       <c r="F380" s="5"/>
       <c r="G380" s="5"/>
     </row>
     <row r="381" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A381" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B381" s="13"/>
+      <c r="C381" s="13"/>
+      <c r="D381" s="13"/>
       <c r="F381" s="5"/>
       <c r="G381" s="5"/>
     </row>
@@ -52203,8 +54919,597 @@
         <v>3.8571836325704827</v>
       </c>
     </row>
+    <row r="434" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A434" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B434" s="13"/>
+      <c r="C434" s="13"/>
+      <c r="D434" s="13"/>
+    </row>
+    <row r="435" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A435" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B435" s="13"/>
+      <c r="C435" s="13"/>
+      <c r="D435" s="13"/>
+    </row>
+    <row r="436" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A436" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B436" t="s">
+        <v>3</v>
+      </c>
+      <c r="C436" t="s">
+        <v>4</v>
+      </c>
+      <c r="D436" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="437" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A437" s="2">
+        <v>8</v>
+      </c>
+      <c r="B437">
+        <v>0</v>
+      </c>
+      <c r="C437">
+        <v>1.2500287500000001E-3</v>
+      </c>
+      <c r="D437">
+        <f>B437/C437</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="438" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A438" s="2">
+        <v>9</v>
+      </c>
+      <c r="B438">
+        <v>0</v>
+      </c>
+      <c r="C438">
+        <v>1.000047E-3</v>
+      </c>
+      <c r="D438">
+        <f t="shared" ref="D438:D473" si="37">B438/C438</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="439" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A439" s="2">
+        <v>10</v>
+      </c>
+      <c r="B439">
+        <v>0</v>
+      </c>
+      <c r="C439">
+        <v>7.5000549999999896E-4</v>
+      </c>
+      <c r="D439">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="440" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A440" s="2">
+        <v>15</v>
+      </c>
+      <c r="B440">
+        <v>0</v>
+      </c>
+      <c r="C440">
+        <v>1.499951E-3</v>
+      </c>
+      <c r="D440">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="441" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A441" s="2">
+        <v>20</v>
+      </c>
+      <c r="B441">
+        <v>0</v>
+      </c>
+      <c r="C441">
+        <v>9.9992774999999902E-4</v>
+      </c>
+      <c r="D441">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="442" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A442" s="2">
+        <v>25</v>
+      </c>
+      <c r="B442">
+        <v>0</v>
+      </c>
+      <c r="C442">
+        <v>9.9998749999999901E-4</v>
+      </c>
+      <c r="D442">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="443" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A443" s="2">
+        <v>30</v>
+      </c>
+      <c r="B443">
+        <v>0</v>
+      </c>
+      <c r="C443">
+        <v>9.9992799999999997E-4</v>
+      </c>
+      <c r="D443">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="444" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A444" s="2">
+        <v>35</v>
+      </c>
+      <c r="B444">
+        <v>0</v>
+      </c>
+      <c r="C444">
+        <v>9.9998749999999901E-4</v>
+      </c>
+      <c r="D444">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="445" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A445" s="2">
+        <v>40</v>
+      </c>
+      <c r="B445">
+        <v>2.4998199999999999E-4</v>
+      </c>
+      <c r="C445">
+        <v>1.000047E-3</v>
+      </c>
+      <c r="D445">
+        <f t="shared" si="37"/>
+        <v>0.24997025139818427</v>
+      </c>
+    </row>
+    <row r="446" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A446" s="2">
+        <v>45</v>
+      </c>
+      <c r="B446">
+        <v>2.4998199999999999E-4</v>
+      </c>
+      <c r="C446">
+        <v>1.000047E-3</v>
+      </c>
+      <c r="D446">
+        <f t="shared" si="37"/>
+        <v>0.24997025139818427</v>
+      </c>
+    </row>
+    <row r="447" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A447" s="2">
+        <v>50</v>
+      </c>
+      <c r="B447">
+        <v>0</v>
+      </c>
+      <c r="C447">
+        <v>9.999875000000001E-4</v>
+      </c>
+      <c r="D447">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="448" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A448" s="2">
+        <v>55</v>
+      </c>
+      <c r="B448">
+        <v>7.5006499999999995E-4</v>
+      </c>
+      <c r="C448">
+        <v>1.2500287500000001E-3</v>
+      </c>
+      <c r="D448">
+        <f t="shared" si="37"/>
+        <v>0.60003819912142009</v>
+      </c>
+    </row>
+    <row r="449" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A449" s="2">
+        <v>60</v>
+      </c>
+      <c r="B449">
+        <v>5.000235E-4</v>
+      </c>
+      <c r="C449">
+        <v>1.0000467499999999E-3</v>
+      </c>
+      <c r="D449">
+        <f t="shared" si="37"/>
+        <v>0.50000012499415658</v>
+      </c>
+    </row>
+    <row r="450" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A450" s="2">
+        <v>65</v>
+      </c>
+      <c r="B450">
+        <v>1.25008825E-3</v>
+      </c>
+      <c r="C450">
+        <v>1.2500287499999901E-3</v>
+      </c>
+      <c r="D450">
+        <f t="shared" si="37"/>
+        <v>1.0000475989052331</v>
+      </c>
+    </row>
+    <row r="451" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A451" s="2">
+        <v>70</v>
+      </c>
+      <c r="B451">
+        <v>1.2500287499999901E-3</v>
+      </c>
+      <c r="C451">
+        <v>1.499951E-3</v>
+      </c>
+      <c r="D451">
+        <f t="shared" si="37"/>
+        <v>0.83337972373763547</v>
+      </c>
+    </row>
+    <row r="452" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A452" s="2">
+        <v>75</v>
+      </c>
+      <c r="B452">
+        <v>1.25008825E-3</v>
+      </c>
+      <c r="C452">
+        <v>1.2499097499999901E-3</v>
+      </c>
+      <c r="D452">
+        <f t="shared" si="37"/>
+        <v>1.0001428103109125</v>
+      </c>
+    </row>
+    <row r="453" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A453" s="2">
+        <v>80</v>
+      </c>
+      <c r="B453">
+        <v>1.74999225E-3</v>
+      </c>
+      <c r="C453">
+        <v>1.24990975E-3</v>
+      </c>
+      <c r="D453">
+        <f t="shared" si="37"/>
+        <v>1.4000948868508305</v>
+      </c>
+    </row>
+    <row r="454" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A454" s="2">
+        <v>85</v>
+      </c>
+      <c r="B454">
+        <v>2.4999380000000002E-3</v>
+      </c>
+      <c r="C454">
+        <v>1.7500517499999999E-3</v>
+      </c>
+      <c r="D454">
+        <f t="shared" si="37"/>
+        <v>1.4284937573988885</v>
+      </c>
+    </row>
+    <row r="455" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A455" s="2">
+        <v>90</v>
+      </c>
+      <c r="B455">
+        <v>2.2500749999999998E-3</v>
+      </c>
+      <c r="C455">
+        <v>1.499951E-3</v>
+      </c>
+      <c r="D455">
+        <f t="shared" si="37"/>
+        <v>1.5000990032341055</v>
+      </c>
+    </row>
+    <row r="456" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A456" s="2">
+        <v>100</v>
+      </c>
+      <c r="B456">
+        <v>3.5000445000000001E-3</v>
+      </c>
+      <c r="C456">
+        <v>1.9999739999999998E-3</v>
+      </c>
+      <c r="D456">
+        <f t="shared" si="37"/>
+        <v>1.7500450005850077</v>
+      </c>
+    </row>
+    <row r="457" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A457" s="2">
+        <v>150</v>
+      </c>
+      <c r="B457">
+        <v>1.4249980250000001E-2</v>
+      </c>
+      <c r="C457">
+        <v>3.7499669999999999E-3</v>
+      </c>
+      <c r="D457">
+        <f t="shared" si="37"/>
+        <v>3.8000281735812611</v>
+      </c>
+    </row>
+    <row r="458" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A458" s="2">
+        <v>200</v>
+      </c>
+      <c r="B458">
+        <v>2.9249965999999999E-2</v>
+      </c>
+      <c r="C458">
+        <v>6.2499640000000002E-3</v>
+      </c>
+      <c r="D458">
+        <f t="shared" si="37"/>
+        <v>4.6800215169239374</v>
+      </c>
+    </row>
+    <row r="459" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A459" s="2">
+        <v>250</v>
+      </c>
+      <c r="B459">
+        <v>5.9499919499999998E-2</v>
+      </c>
+      <c r="C459">
+        <v>1.34999749999999E-2</v>
+      </c>
+      <c r="D459">
+        <f t="shared" si="37"/>
+        <v>4.4074096063141184</v>
+      </c>
+    </row>
+    <row r="460" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A460" s="2">
+        <v>300</v>
+      </c>
+      <c r="B460">
+        <v>0.10400003225</v>
+      </c>
+      <c r="C460">
+        <v>2.1500050999999999E-2</v>
+      </c>
+      <c r="D460">
+        <f t="shared" si="37"/>
+        <v>4.8371993280388033</v>
+      </c>
+    </row>
+    <row r="461" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A461" s="2">
+        <v>350</v>
+      </c>
+      <c r="B461">
+        <v>0.16900002949999901</v>
+      </c>
+      <c r="C461">
+        <v>3.374993775E-2</v>
+      </c>
+      <c r="D461">
+        <f t="shared" si="37"/>
+        <v>5.007417517384873</v>
+      </c>
+    </row>
+    <row r="462" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A462" s="2">
+        <v>400</v>
+      </c>
+      <c r="B462">
+        <v>0.26800000624999998</v>
+      </c>
+      <c r="C462">
+        <v>5.3999960249999999E-2</v>
+      </c>
+      <c r="D462">
+        <f t="shared" si="37"/>
+        <v>4.9629667319986588</v>
+      </c>
+    </row>
+    <row r="463" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A463" s="2">
+        <v>450</v>
+      </c>
+      <c r="B463">
+        <v>0.49374997599999898</v>
+      </c>
+      <c r="C463">
+        <v>8.4249913750000002E-2</v>
+      </c>
+      <c r="D463">
+        <f t="shared" si="37"/>
+        <v>5.8605398394250461</v>
+      </c>
+    </row>
+    <row r="464" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A464" s="2">
+        <v>500</v>
+      </c>
+      <c r="B464">
+        <v>0.61200004824999998</v>
+      </c>
+      <c r="C464">
+        <v>0.105749965</v>
+      </c>
+      <c r="D464">
+        <f t="shared" si="37"/>
+        <v>5.7872364142153616</v>
+      </c>
+    </row>
+    <row r="465" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A465" s="2">
+        <v>550</v>
+      </c>
+      <c r="B465">
+        <v>0.80424994225000002</v>
+      </c>
+      <c r="C465">
+        <v>0.15300005649999901</v>
+      </c>
+      <c r="D465">
+        <f t="shared" si="37"/>
+        <v>5.2565336291232363</v>
+      </c>
+    </row>
+    <row r="466" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A466" s="2">
+        <v>600</v>
+      </c>
+      <c r="B466">
+        <v>1.0489999652499999</v>
+      </c>
+      <c r="C466">
+        <v>0.192999959</v>
+      </c>
+      <c r="D466">
+        <f t="shared" si="37"/>
+        <v>5.435234135205179</v>
+      </c>
+    </row>
+    <row r="467" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A467" s="2">
+        <v>650</v>
+      </c>
+      <c r="B467">
+        <v>1.28225010625</v>
+      </c>
+      <c r="C467">
+        <v>0.24175000175</v>
+      </c>
+      <c r="D467">
+        <f t="shared" si="37"/>
+        <v>5.3040334931455693</v>
+      </c>
+    </row>
+    <row r="468" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A468" s="2">
+        <v>700</v>
+      </c>
+      <c r="B468">
+        <v>1.8015000225</v>
+      </c>
+      <c r="C468">
+        <v>0.296249926</v>
+      </c>
+      <c r="D468">
+        <f t="shared" si="37"/>
+        <v>6.0810142531478641</v>
+      </c>
+    </row>
+    <row r="469" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A469" s="2">
+        <v>750</v>
+      </c>
+      <c r="B469">
+        <v>2.1537499425000002</v>
+      </c>
+      <c r="C469">
+        <v>0.38100004199999998</v>
+      </c>
+      <c r="D469">
+        <f t="shared" si="37"/>
+        <v>5.6528863650361494</v>
+      </c>
+    </row>
+    <row r="470" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A470" s="2">
+        <v>800</v>
+      </c>
+      <c r="B470">
+        <v>2.4997500179999999</v>
+      </c>
+      <c r="C470">
+        <v>0.467999994999999</v>
+      </c>
+      <c r="D470">
+        <f t="shared" si="37"/>
+        <v>5.3413462493733688</v>
+      </c>
+    </row>
+    <row r="471" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A471" s="2">
+        <v>850</v>
+      </c>
+      <c r="B471">
+        <v>3.0032498834999899</v>
+      </c>
+      <c r="C471">
+        <v>0.55200004574999995</v>
+      </c>
+      <c r="D471">
+        <f t="shared" si="37"/>
+        <v>5.4406696278792657</v>
+      </c>
+    </row>
+    <row r="472" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A472" s="2">
+        <v>900</v>
+      </c>
+      <c r="B472">
+        <v>3.62575000525</v>
+      </c>
+      <c r="C472">
+        <v>0.70500004299999997</v>
+      </c>
+      <c r="D472">
+        <f t="shared" si="37"/>
+        <v>5.1429074951843656</v>
+      </c>
+    </row>
+    <row r="473" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A473" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B473">
+        <v>5.3065000177499897</v>
+      </c>
+      <c r="C473">
+        <v>1.13124996425</v>
+      </c>
+      <c r="D473">
+        <f t="shared" si="37"/>
+        <v>4.6908288932129256</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="11">
+    <mergeCell ref="A380:D380"/>
+    <mergeCell ref="A381:D381"/>
+    <mergeCell ref="A434:D434"/>
+    <mergeCell ref="A435:D435"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="M1:Q1"/>
     <mergeCell ref="I2:K2"/>

</xml_diff>